<commit_message>
Icing On The Cake
</commit_message>
<xml_diff>
--- a/Document/DXTBidMasters Master Schedule.xlsx
+++ b/Document/DXTBidMasters Master Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT\Compe\HackAIthon 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C5BE52-78C7-472A-BCAF-2369D79F9CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D092D1-7BDE-4693-954E-A5B3E7C8D30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="holidays">#REF!</definedName>
     <definedName name="no_of_workingday">IF(OR(ISBLANK('Master Plan'!task_start),ISBLANK('Master Plan'!task_end)),"",NETWORKDAYS('Master Plan'!task_start,'Master Plan'!task_end,holidays))</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Master Plan'!$1:$16</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Master Plan'!$1:$52</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Master Plan'!$4:$6</definedName>
     <definedName name="task_end" localSheetId="0">'Master Plan'!$E1</definedName>
     <definedName name="task_progress" localSheetId="0">'Master Plan'!$C1</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Project Start:</t>
   </si>
@@ -74,34 +74,142 @@
     <t>Plan end</t>
   </si>
   <si>
-    <t>4. Documentation</t>
+    <t>1. Backend &amp; Cloud Hosting</t>
   </si>
   <si>
-    <t>3. AI and Prompt Engineering</t>
+    <t>2. Frontend Development</t>
   </si>
   <si>
-    <t>4.1 High-level Architecture</t>
+    <t>2.1 Setup Simple UI</t>
   </si>
   <si>
-    <t>4.2 Problem Statement</t>
+    <t>2.2 Make a Simple Flow for Creating a Roadmap</t>
   </si>
   <si>
-    <t>3. Frontend Development</t>
+    <t>3. Documentation</t>
   </si>
   <si>
-    <t>3.1 Simple Tree Output</t>
+    <t>3.1 Topic Analysis</t>
   </si>
   <si>
-    <t>2. Backend &amp; Cloud Hosting</t>
+    <t>3.2 Business Analysis Documents</t>
   </si>
   <si>
-    <t>2.1 Backend Development</t>
+    <t>3.3 High-level Architecture</t>
   </si>
   <si>
-    <t>2.2 Setup Services</t>
+    <t>3.4 Mapping AI Models</t>
   </si>
   <si>
-    <t>3.1 Setup Simple Flow</t>
+    <t>3.5 Make and update slides</t>
+  </si>
+  <si>
+    <t>3.6 List Out All Features</t>
+  </si>
+  <si>
+    <t>3.7 Mapping Features with Actual UI</t>
+  </si>
+  <si>
+    <t>4. AI and Prompt Engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       4.1 Find Suitable Models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       4.2 Verify Suitable Models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       4.3 Find AI tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       4.4 AI Usage Statistic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  4.5 Research &amp; Integrate RAG</t>
+  </si>
+  <si>
+    <t>2.3 Setup Flow Analyzing from Profile</t>
+  </si>
+  <si>
+    <t>2.4 Dashboard with Roadmaps Indicated as Cards</t>
+  </si>
+  <si>
+    <t>2.5 Integrate with Backend API</t>
+  </si>
+  <si>
+    <t>2.6 Setup Profile Page</t>
+  </si>
+  <si>
+    <t>2.7 Roadmap Detail</t>
+  </si>
+  <si>
+    <t>2.8 Generate Node Based UI</t>
+  </si>
+  <si>
+    <t>2.9 Host on Vercel</t>
+  </si>
+  <si>
+    <t>2.10 Validate from Frontend</t>
+  </si>
+  <si>
+    <t>3.8 User Journey</t>
+  </si>
+  <si>
+    <t>3.9 High-level Cloud Infrastructure</t>
+  </si>
+  <si>
+    <t>3.10 Mapping Features with Objects</t>
+  </si>
+  <si>
+    <t>3.11 Make SRS Document</t>
+  </si>
+  <si>
+    <t>1.1 Implement Google Prompt Module</t>
+  </si>
+  <si>
+    <t>1.2 Integrate with AI API</t>
+  </si>
+  <si>
+    <t>1.3 POST Goal</t>
+  </si>
+  <si>
+    <t>1.4 GET Related Skills</t>
+  </si>
+  <si>
+    <t>1.5 POST Manually Checked Skills</t>
+  </si>
+  <si>
+    <t>1.6 Make a Database</t>
+  </si>
+  <si>
+    <t>1.7 Make Python Service</t>
+  </si>
+  <si>
+    <t>1.8 GET Roadmap Detail</t>
+  </si>
+  <si>
+    <t>1.9 POST Assess from Profile</t>
+  </si>
+  <si>
+    <t>1.10 GET Personal Information</t>
+  </si>
+  <si>
+    <t>1.11 GET Existing Roadmaps</t>
+  </si>
+  <si>
+    <t>1.12 Update Roadmap If Changes Occurred In DB</t>
+  </si>
+  <si>
+    <t>1.13 Integrate Main Backend with Embedding Service</t>
+  </si>
+  <si>
+    <t>1.14 Make Chat Service</t>
+  </si>
+  <si>
+    <t>1.15 Setup AWS</t>
+  </si>
+  <si>
+    <t>1.16 Reboot the Auth Service</t>
   </si>
 </sst>
 </file>
@@ -252,7 +360,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -537,21 +645,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -637,9 +730,7 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -652,12 +743,36 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -670,7 +785,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -766,14 +881,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -789,11 +904,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="5" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -803,6 +928,12 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -838,7 +969,7 @@
     <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="58">
     <dxf>
       <font>
         <b/>
@@ -855,47 +986,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -941,37 +1031,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -988,44 +1047,18 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFC7CE"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="8" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="8" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFFF0000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFF0000"/>
+        </right>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1073,6 +1106,13 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1089,30 +1129,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
@@ -1134,6 +1150,13 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1149,43 +1172,9 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
       <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.39997558519241921"/>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1206,6 +1195,199 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFC7CE"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFFF0000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFF0000"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFC7CE"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFFF0000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFF0000"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFC7CE"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFFF0000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFF0000"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFC7CE"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFFF0000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFF0000"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <bgColor theme="8" tint="0.59999389629810485"/>
         </patternFill>
@@ -1213,10 +1395,32 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59999389629810485"/>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFC7CE"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFFF0000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFF0000"/>
+        </right>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1229,21 +1433,57 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="0"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="8" tint="-0.249977111117893"/>
+          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFC7CE"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFFF0000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFF0000"/>
+        </right>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1356,15 +1596,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="49"/>
-      <tableStyleElement type="headerRow" dxfId="48"/>
-      <tableStyleElement type="totalRow" dxfId="47"/>
-      <tableStyleElement type="firstColumn" dxfId="46"/>
-      <tableStyleElement type="lastColumn" dxfId="45"/>
-      <tableStyleElement type="firstRowStripe" dxfId="44"/>
-      <tableStyleElement type="secondRowStripe" dxfId="43"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="42"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="41"/>
+      <tableStyleElement type="wholeTable" dxfId="57"/>
+      <tableStyleElement type="headerRow" dxfId="56"/>
+      <tableStyleElement type="totalRow" dxfId="55"/>
+      <tableStyleElement type="firstColumn" dxfId="54"/>
+      <tableStyleElement type="lastColumn" dxfId="53"/>
+      <tableStyleElement type="firstRowStripe" dxfId="52"/>
+      <tableStyleElement type="secondRowStripe" dxfId="51"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="50"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="49"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1724,11 +1964,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AU17"/>
+  <dimension ref="A1:AU53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="90" zoomScaleNormal="60" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W13" sqref="W13"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1754,55 +1994,55 @@
       <c r="D1" s="2"/>
       <c r="E1" s="7"/>
       <c r="F1" s="4"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="57"/>
-      <c r="V1" s="57"/>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="63"/>
+      <c r="X1" s="63"/>
     </row>
     <row r="2" spans="1:47" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="51">
+      <c r="D2" s="57">
         <v>45803</v>
       </c>
-      <c r="E2" s="52"/>
-      <c r="G2" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
+      <c r="E2" s="58"/>
+      <c r="G2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="O2" s="61"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
       <c r="U2" s="8"/>
     </row>
     <row r="3" spans="1:47" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="51">
+      <c r="D3" s="57">
         <f ca="1">TODAY()</f>
-        <v>45811</v>
-      </c>
-      <c r="E3" s="52"/>
+        <v>45820</v>
+      </c>
+      <c r="E3" s="58"/>
     </row>
     <row r="4" spans="1:47" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="18" t="s">
@@ -1811,66 +2051,66 @@
       <c r="D4" s="9">
         <v>0</v>
       </c>
-      <c r="F4" s="58">
+      <c r="F4" s="64">
         <f>F5</f>
         <v>45796</v>
       </c>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="56">
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="62">
         <f t="shared" ref="M4" si="0">M5</f>
         <v>45803</v>
       </c>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="56"/>
-      <c r="S4" s="56"/>
-      <c r="T4" s="56">
+      <c r="N4" s="62"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="62"/>
+      <c r="Q4" s="62"/>
+      <c r="R4" s="62"/>
+      <c r="S4" s="62"/>
+      <c r="T4" s="62">
         <f t="shared" ref="T4" si="1">T5</f>
         <v>45810</v>
       </c>
-      <c r="U4" s="56"/>
-      <c r="V4" s="56"/>
-      <c r="W4" s="56"/>
-      <c r="X4" s="56"/>
-      <c r="Y4" s="56"/>
-      <c r="Z4" s="56"/>
-      <c r="AA4" s="56">
+      <c r="U4" s="62"/>
+      <c r="V4" s="62"/>
+      <c r="W4" s="62"/>
+      <c r="X4" s="62"/>
+      <c r="Y4" s="62"/>
+      <c r="Z4" s="62"/>
+      <c r="AA4" s="62">
         <f t="shared" ref="AA4" si="2">AA5</f>
         <v>45817</v>
       </c>
-      <c r="AB4" s="56"/>
-      <c r="AC4" s="56"/>
-      <c r="AD4" s="56"/>
-      <c r="AE4" s="56"/>
-      <c r="AF4" s="56"/>
-      <c r="AG4" s="56"/>
-      <c r="AH4" s="56">
+      <c r="AB4" s="62"/>
+      <c r="AC4" s="62"/>
+      <c r="AD4" s="62"/>
+      <c r="AE4" s="62"/>
+      <c r="AF4" s="62"/>
+      <c r="AG4" s="62"/>
+      <c r="AH4" s="62">
         <f t="shared" ref="AH4" si="3">AH5</f>
         <v>45824</v>
       </c>
-      <c r="AI4" s="56"/>
-      <c r="AJ4" s="56"/>
-      <c r="AK4" s="56"/>
-      <c r="AL4" s="56"/>
-      <c r="AM4" s="56"/>
-      <c r="AN4" s="56"/>
-      <c r="AO4" s="56">
+      <c r="AI4" s="62"/>
+      <c r="AJ4" s="62"/>
+      <c r="AK4" s="62"/>
+      <c r="AL4" s="62"/>
+      <c r="AM4" s="62"/>
+      <c r="AN4" s="62"/>
+      <c r="AO4" s="62">
         <f t="shared" ref="AO4" si="4">AO5</f>
         <v>45831</v>
       </c>
-      <c r="AP4" s="56"/>
-      <c r="AQ4" s="56"/>
-      <c r="AR4" s="56"/>
-      <c r="AS4" s="56"/>
-      <c r="AT4" s="56"/>
-      <c r="AU4" s="56"/>
+      <c r="AP4" s="62"/>
+      <c r="AQ4" s="62"/>
+      <c r="AR4" s="62"/>
+      <c r="AS4" s="62"/>
+      <c r="AT4" s="62"/>
+      <c r="AU4" s="62"/>
     </row>
     <row r="5" spans="1:47" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D5" s="3"/>
@@ -2230,22 +2470,22 @@
     </row>
     <row r="7" spans="1:47" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="34" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7" s="19">
         <v>1</v>
       </c>
       <c r="C7" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="13">
         <v>45810</v>
       </c>
       <c r="E7" s="13">
-        <v>45816</v>
+        <v>45819</v>
       </c>
       <c r="F7" s="11" t="str">
-        <f t="shared" ref="F7:L11" ca="1" si="15">IF(AND(F$5&gt;$E7,$C7&lt;100%,F$5&lt;=TODAY()),"D","")</f>
+        <f t="shared" ref="F7:L34" ca="1" si="15">IF(AND(F$5&gt;$E7,$C7&lt;100%,F$5&lt;=TODAY()),"D","")</f>
         <v/>
       </c>
       <c r="G7" s="11" t="str">
@@ -2310,19 +2550,19 @@
     </row>
     <row r="8" spans="1:47" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B8" s="19">
         <v>1</v>
       </c>
       <c r="C8" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="13">
-        <v>45810</v>
+        <v>45813</v>
       </c>
       <c r="E8" s="13">
-        <v>45816</v>
+        <v>45813</v>
       </c>
       <c r="F8" s="11" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -2367,7 +2607,7 @@
       <c r="Y8" s="11"/>
       <c r="Z8" s="11"/>
       <c r="AA8" s="11"/>
-      <c r="AB8" s="40"/>
+      <c r="AB8" s="39"/>
       <c r="AC8" s="11"/>
       <c r="AD8" s="11"/>
       <c r="AE8" s="11"/>
@@ -2390,19 +2630,19 @@
     </row>
     <row r="9" spans="1:47" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B9" s="19">
         <v>1</v>
       </c>
       <c r="C9" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="13">
-        <v>45812</v>
+        <v>45813</v>
       </c>
       <c r="E9" s="13">
-        <v>45812</v>
+        <v>45813</v>
       </c>
       <c r="F9" s="11" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -2447,7 +2687,7 @@
       <c r="Y9" s="11"/>
       <c r="Z9" s="11"/>
       <c r="AA9" s="11"/>
-      <c r="AB9" s="40"/>
+      <c r="AB9" s="39"/>
       <c r="AC9" s="11"/>
       <c r="AD9" s="11"/>
       <c r="AE9" s="11"/>
@@ -2468,21 +2708,21 @@
       <c r="AT9" s="11"/>
       <c r="AU9" s="25"/>
     </row>
-    <row r="10" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="20">
-        <v>10.8</v>
+    <row r="10" spans="1:47" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="19">
+        <v>1</v>
       </c>
       <c r="C10" s="12">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="13">
-        <v>45809</v>
+        <v>45814</v>
       </c>
       <c r="E10" s="13">
-        <v>45816</v>
+        <v>45814</v>
       </c>
       <c r="F10" s="11" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -2513,23 +2753,56 @@
         <v/>
       </c>
       <c r="M10" s="24"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="39"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="11"/>
+      <c r="AG10" s="11"/>
+      <c r="AH10" s="11"/>
+      <c r="AI10" s="11"/>
+      <c r="AJ10" s="11"/>
+      <c r="AK10" s="11"/>
+      <c r="AL10" s="11"/>
+      <c r="AM10" s="11"/>
+      <c r="AN10" s="11"/>
+      <c r="AO10" s="11"/>
+      <c r="AP10" s="11"/>
+      <c r="AQ10" s="11"/>
+      <c r="AR10" s="11"/>
+      <c r="AS10" s="11"/>
+      <c r="AT10" s="11"/>
       <c r="AU10" s="25"/>
     </row>
-    <row r="11" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="20">
-        <v>10.8</v>
+        <v>42</v>
+      </c>
+      <c r="B11" s="19">
+        <v>1</v>
       </c>
       <c r="C11" s="12">
         <v>1</v>
       </c>
       <c r="D11" s="13">
-        <v>45809</v>
+        <v>45814</v>
       </c>
       <c r="E11" s="13">
-        <v>45811</v>
+        <v>45814</v>
       </c>
       <c r="F11" s="11" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -2560,105 +2833,204 @@
         <v/>
       </c>
       <c r="M11" s="24"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="39"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="11"/>
+      <c r="AE11" s="11"/>
+      <c r="AF11" s="11"/>
+      <c r="AG11" s="11"/>
+      <c r="AH11" s="11"/>
+      <c r="AI11" s="11"/>
+      <c r="AJ11" s="11"/>
+      <c r="AK11" s="11"/>
+      <c r="AL11" s="11"/>
+      <c r="AM11" s="11"/>
+      <c r="AN11" s="11"/>
+      <c r="AO11" s="11"/>
+      <c r="AP11" s="11"/>
+      <c r="AQ11" s="11"/>
+      <c r="AR11" s="11"/>
+      <c r="AS11" s="11"/>
+      <c r="AT11" s="11"/>
       <c r="AU11" s="25"/>
     </row>
-    <row r="12" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="34" t="s">
-        <v>9</v>
+    <row r="12" spans="1:47" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="36" t="s">
+        <v>43</v>
       </c>
       <c r="B12" s="19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C12" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="13">
-        <v>45807</v>
+        <v>45816</v>
       </c>
       <c r="E12" s="13">
-        <v>45810</v>
+        <v>45816</v>
       </c>
       <c r="F12" s="11" t="str">
-        <f t="shared" ref="F12:L13" ca="1" si="16">IF(AND(F$5&gt;$E12,$C12&lt;100%,F$5&lt;=TODAY()),"D","")</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="G12" s="11" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="H12" s="11" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="I12" s="11" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="J12" s="11" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="K12" s="11" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="L12" s="11" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="M12" s="24"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="11"/>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="39"/>
+      <c r="AC12" s="11"/>
+      <c r="AD12" s="11"/>
+      <c r="AE12" s="11"/>
+      <c r="AF12" s="11"/>
+      <c r="AG12" s="11"/>
+      <c r="AH12" s="11"/>
+      <c r="AI12" s="11"/>
+      <c r="AJ12" s="11"/>
+      <c r="AK12" s="11"/>
+      <c r="AL12" s="11"/>
+      <c r="AM12" s="11"/>
+      <c r="AN12" s="11"/>
+      <c r="AO12" s="11"/>
+      <c r="AP12" s="11"/>
+      <c r="AQ12" s="11"/>
+      <c r="AR12" s="11"/>
+      <c r="AS12" s="11"/>
+      <c r="AT12" s="11"/>
       <c r="AU12" s="25"/>
     </row>
-    <row r="13" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:47" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B13" s="19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" s="12">
         <v>1</v>
       </c>
       <c r="D13" s="13">
-        <v>45810</v>
+        <v>45816</v>
       </c>
       <c r="E13" s="13">
-        <v>45810</v>
+        <v>45816</v>
       </c>
       <c r="F13" s="11" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="G13" s="11" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="H13" s="11" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="I13" s="11" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="J13" s="11" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="K13" s="11" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="L13" s="11" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="M13" s="24"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="11"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="39"/>
+      <c r="AC13" s="11"/>
+      <c r="AD13" s="11"/>
+      <c r="AE13" s="11"/>
+      <c r="AF13" s="11"/>
+      <c r="AG13" s="11"/>
+      <c r="AH13" s="11"/>
+      <c r="AI13" s="11"/>
+      <c r="AJ13" s="11"/>
+      <c r="AK13" s="11"/>
+      <c r="AL13" s="11"/>
+      <c r="AM13" s="11"/>
+      <c r="AN13" s="11"/>
+      <c r="AO13" s="11"/>
+      <c r="AP13" s="11"/>
+      <c r="AQ13" s="11"/>
+      <c r="AR13" s="11"/>
+      <c r="AS13" s="11"/>
+      <c r="AT13" s="11"/>
       <c r="AU13" s="25"/>
     </row>
-    <row r="14" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:47" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="36" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B14" s="19">
         <v>1</v>
@@ -2667,176 +3039,1936 @@
         <v>1</v>
       </c>
       <c r="D14" s="13">
-        <v>45807</v>
+        <v>45815</v>
       </c>
       <c r="E14" s="13">
-        <v>45807</v>
+        <v>45816</v>
+      </c>
+      <c r="F14" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="G14" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="H14" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="I14" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="J14" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="K14" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="L14" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
       </c>
       <c r="M14" s="24"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="39"/>
+      <c r="AC14" s="11"/>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="11"/>
+      <c r="AF14" s="11"/>
+      <c r="AG14" s="11"/>
+      <c r="AH14" s="11"/>
+      <c r="AI14" s="11"/>
+      <c r="AJ14" s="11"/>
+      <c r="AK14" s="11"/>
+      <c r="AL14" s="11"/>
+      <c r="AM14" s="11"/>
+      <c r="AN14" s="11"/>
+      <c r="AO14" s="11"/>
+      <c r="AP14" s="11"/>
+      <c r="AQ14" s="11"/>
+      <c r="AR14" s="11"/>
+      <c r="AS14" s="11"/>
+      <c r="AT14" s="11"/>
       <c r="AU14" s="25"/>
     </row>
-    <row r="15" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="35" t="s">
+    <row r="15" spans="1:47" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="19">
+        <v>1</v>
+      </c>
+      <c r="C15" s="12">
+        <v>1</v>
+      </c>
+      <c r="D15" s="13">
+        <v>45817</v>
+      </c>
+      <c r="E15" s="13">
+        <v>45817</v>
+      </c>
+      <c r="F15" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="G15" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="H15" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="I15" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="J15" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="K15" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="L15" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="M15" s="24"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="39"/>
+      <c r="AC15" s="11"/>
+      <c r="AD15" s="11"/>
+      <c r="AE15" s="11"/>
+      <c r="AF15" s="11"/>
+      <c r="AG15" s="11"/>
+      <c r="AH15" s="11"/>
+      <c r="AI15" s="11"/>
+      <c r="AJ15" s="11"/>
+      <c r="AK15" s="11"/>
+      <c r="AL15" s="11"/>
+      <c r="AM15" s="11"/>
+      <c r="AN15" s="11"/>
+      <c r="AO15" s="11"/>
+      <c r="AP15" s="11"/>
+      <c r="AQ15" s="11"/>
+      <c r="AR15" s="11"/>
+      <c r="AS15" s="11"/>
+      <c r="AT15" s="11"/>
+      <c r="AU15" s="25"/>
+    </row>
+    <row r="16" spans="1:47" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="19">
+        <v>1</v>
+      </c>
+      <c r="C16" s="12">
+        <v>1</v>
+      </c>
+      <c r="D16" s="13">
+        <v>45817</v>
+      </c>
+      <c r="E16" s="13">
+        <v>45817</v>
+      </c>
+      <c r="F16" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="G16" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="H16" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="I16" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="J16" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="K16" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="L16" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="M16" s="24"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="11"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="39"/>
+      <c r="AC16" s="11"/>
+      <c r="AD16" s="11"/>
+      <c r="AE16" s="11"/>
+      <c r="AF16" s="11"/>
+      <c r="AG16" s="11"/>
+      <c r="AH16" s="11"/>
+      <c r="AI16" s="11"/>
+      <c r="AJ16" s="11"/>
+      <c r="AK16" s="11"/>
+      <c r="AL16" s="11"/>
+      <c r="AM16" s="11"/>
+      <c r="AN16" s="11"/>
+      <c r="AO16" s="11"/>
+      <c r="AP16" s="11"/>
+      <c r="AQ16" s="11"/>
+      <c r="AR16" s="11"/>
+      <c r="AS16" s="11"/>
+      <c r="AT16" s="11"/>
+      <c r="AU16" s="25"/>
+    </row>
+    <row r="17" spans="1:47" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="19">
+        <v>1</v>
+      </c>
+      <c r="C17" s="12">
+        <v>1</v>
+      </c>
+      <c r="D17" s="13">
+        <v>45817</v>
+      </c>
+      <c r="E17" s="13">
+        <v>45817</v>
+      </c>
+      <c r="F17" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="G17" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="H17" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="I17" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="J17" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="K17" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="L17" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="M17" s="24"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="11"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="39"/>
+      <c r="AC17" s="11"/>
+      <c r="AD17" s="11"/>
+      <c r="AE17" s="11"/>
+      <c r="AF17" s="11"/>
+      <c r="AG17" s="11"/>
+      <c r="AH17" s="11"/>
+      <c r="AI17" s="11"/>
+      <c r="AJ17" s="11"/>
+      <c r="AK17" s="11"/>
+      <c r="AL17" s="11"/>
+      <c r="AM17" s="11"/>
+      <c r="AN17" s="11"/>
+      <c r="AO17" s="11"/>
+      <c r="AP17" s="11"/>
+      <c r="AQ17" s="11"/>
+      <c r="AR17" s="11"/>
+      <c r="AS17" s="11"/>
+      <c r="AT17" s="11"/>
+      <c r="AU17" s="25"/>
+    </row>
+    <row r="18" spans="1:47" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="12">
+        <v>1</v>
+      </c>
+      <c r="D18" s="13">
+        <v>45817</v>
+      </c>
+      <c r="E18" s="13">
+        <v>45817</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="39"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="11"/>
+      <c r="AE18" s="11"/>
+      <c r="AF18" s="11"/>
+      <c r="AG18" s="11"/>
+      <c r="AH18" s="11"/>
+      <c r="AI18" s="11"/>
+      <c r="AJ18" s="11"/>
+      <c r="AK18" s="11"/>
+      <c r="AL18" s="11"/>
+      <c r="AM18" s="11"/>
+      <c r="AN18" s="11"/>
+      <c r="AO18" s="11"/>
+      <c r="AP18" s="11"/>
+      <c r="AQ18" s="11"/>
+      <c r="AR18" s="11"/>
+      <c r="AS18" s="11"/>
+      <c r="AT18" s="11"/>
+      <c r="AU18" s="25"/>
+    </row>
+    <row r="19" spans="1:47" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="12">
+        <v>1</v>
+      </c>
+      <c r="D19" s="13">
+        <v>45815</v>
+      </c>
+      <c r="E19" s="13">
+        <v>45818</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="39"/>
+      <c r="AC19" s="11"/>
+      <c r="AD19" s="11"/>
+      <c r="AE19" s="11"/>
+      <c r="AF19" s="11"/>
+      <c r="AG19" s="11"/>
+      <c r="AH19" s="11"/>
+      <c r="AI19" s="11"/>
+      <c r="AJ19" s="11"/>
+      <c r="AK19" s="11"/>
+      <c r="AL19" s="11"/>
+      <c r="AM19" s="11"/>
+      <c r="AN19" s="11"/>
+      <c r="AO19" s="11"/>
+      <c r="AP19" s="11"/>
+      <c r="AQ19" s="11"/>
+      <c r="AR19" s="11"/>
+      <c r="AS19" s="11"/>
+      <c r="AT19" s="11"/>
+      <c r="AU19" s="25"/>
+    </row>
+    <row r="20" spans="1:47" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="19">
+        <v>1</v>
+      </c>
+      <c r="C20" s="12">
+        <v>1</v>
+      </c>
+      <c r="D20" s="13">
+        <v>45819</v>
+      </c>
+      <c r="E20" s="13">
+        <v>45819</v>
+      </c>
+      <c r="F20" s="11" t="str">
+        <f t="shared" ref="F20:L23" ca="1" si="16">IF(AND(F$5&gt;$E20,$C20&lt;100%,F$5&lt;=TODAY()),"D","")</f>
+        <v/>
+      </c>
+      <c r="G20" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="H20" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="I20" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="J20" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="K20" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="L20" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="M20" s="24"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="11"/>
+      <c r="AB20" s="39"/>
+      <c r="AC20" s="11"/>
+      <c r="AD20" s="11"/>
+      <c r="AE20" s="11"/>
+      <c r="AF20" s="11"/>
+      <c r="AG20" s="11"/>
+      <c r="AH20" s="11"/>
+      <c r="AI20" s="11"/>
+      <c r="AJ20" s="11"/>
+      <c r="AK20" s="11"/>
+      <c r="AL20" s="11"/>
+      <c r="AM20" s="11"/>
+      <c r="AN20" s="11"/>
+      <c r="AO20" s="11"/>
+      <c r="AP20" s="11"/>
+      <c r="AQ20" s="11"/>
+      <c r="AR20" s="11"/>
+      <c r="AS20" s="11"/>
+      <c r="AT20" s="11"/>
+      <c r="AU20" s="25"/>
+    </row>
+    <row r="21" spans="1:47" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="19">
+        <v>1</v>
+      </c>
+      <c r="C21" s="12">
+        <v>1</v>
+      </c>
+      <c r="D21" s="13">
+        <v>45816</v>
+      </c>
+      <c r="E21" s="13">
+        <v>45819</v>
+      </c>
+      <c r="F21" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="G21" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="H21" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="I21" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="J21" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="K21" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="L21" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="M21" s="24"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="11"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="39"/>
+      <c r="AC21" s="11"/>
+      <c r="AD21" s="11"/>
+      <c r="AE21" s="11"/>
+      <c r="AF21" s="11"/>
+      <c r="AG21" s="11"/>
+      <c r="AH21" s="11"/>
+      <c r="AI21" s="11"/>
+      <c r="AJ21" s="11"/>
+      <c r="AK21" s="11"/>
+      <c r="AL21" s="11"/>
+      <c r="AM21" s="11"/>
+      <c r="AN21" s="11"/>
+      <c r="AO21" s="11"/>
+      <c r="AP21" s="11"/>
+      <c r="AQ21" s="11"/>
+      <c r="AR21" s="11"/>
+      <c r="AS21" s="11"/>
+      <c r="AT21" s="11"/>
+      <c r="AU21" s="25"/>
+    </row>
+    <row r="22" spans="1:47" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="19">
+        <v>1</v>
+      </c>
+      <c r="C22" s="12">
+        <v>1</v>
+      </c>
+      <c r="D22" s="13">
+        <v>45819</v>
+      </c>
+      <c r="E22" s="13">
+        <v>45819</v>
+      </c>
+      <c r="F22" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="G22" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="H22" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="I22" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="J22" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="K22" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="L22" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="M22" s="24"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+      <c r="X22" s="11"/>
+      <c r="Y22" s="11"/>
+      <c r="Z22" s="11"/>
+      <c r="AA22" s="11"/>
+      <c r="AB22" s="39"/>
+      <c r="AC22" s="11"/>
+      <c r="AD22" s="11"/>
+      <c r="AE22" s="11"/>
+      <c r="AF22" s="11"/>
+      <c r="AG22" s="11"/>
+      <c r="AH22" s="11"/>
+      <c r="AI22" s="11"/>
+      <c r="AJ22" s="11"/>
+      <c r="AK22" s="11"/>
+      <c r="AL22" s="11"/>
+      <c r="AM22" s="11"/>
+      <c r="AN22" s="11"/>
+      <c r="AO22" s="11"/>
+      <c r="AP22" s="11"/>
+      <c r="AQ22" s="11"/>
+      <c r="AR22" s="11"/>
+      <c r="AS22" s="11"/>
+      <c r="AT22" s="11"/>
+      <c r="AU22" s="25"/>
+    </row>
+    <row r="23" spans="1:47" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="19">
+        <v>1</v>
+      </c>
+      <c r="C23" s="12">
+        <v>1</v>
+      </c>
+      <c r="D23" s="13">
+        <v>45819</v>
+      </c>
+      <c r="E23" s="13">
+        <v>45819</v>
+      </c>
+      <c r="F23" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="G23" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="H23" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="I23" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="J23" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="K23" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="L23" s="11" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v/>
+      </c>
+      <c r="M23" s="24"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="11"/>
+      <c r="AB23" s="39"/>
+      <c r="AC23" s="11"/>
+      <c r="AD23" s="11"/>
+      <c r="AE23" s="11"/>
+      <c r="AF23" s="11"/>
+      <c r="AG23" s="11"/>
+      <c r="AH23" s="11"/>
+      <c r="AI23" s="11"/>
+      <c r="AJ23" s="11"/>
+      <c r="AK23" s="11"/>
+      <c r="AL23" s="11"/>
+      <c r="AM23" s="11"/>
+      <c r="AN23" s="11"/>
+      <c r="AO23" s="11"/>
+      <c r="AP23" s="11"/>
+      <c r="AQ23" s="11"/>
+      <c r="AR23" s="11"/>
+      <c r="AS23" s="11"/>
+      <c r="AT23" s="11"/>
+      <c r="AU23" s="25"/>
+    </row>
+    <row r="24" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="12">
-        <v>0</v>
-      </c>
-      <c r="D15" s="13">
+      <c r="B24" s="20">
+        <v>10.8</v>
+      </c>
+      <c r="C24" s="12">
+        <v>1</v>
+      </c>
+      <c r="D24" s="13">
+        <v>45809</v>
+      </c>
+      <c r="E24" s="13">
+        <v>45819</v>
+      </c>
+      <c r="F24" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="G24" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="H24" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="I24" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="J24" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="K24" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="L24" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="M24" s="24"/>
+      <c r="AU24" s="25"/>
+    </row>
+    <row r="25" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="20">
+        <v>10.8</v>
+      </c>
+      <c r="C25" s="12">
+        <v>1</v>
+      </c>
+      <c r="D25" s="13">
         <v>45810</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E25" s="13">
+        <v>45812</v>
+      </c>
+      <c r="F25" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="G25" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="H25" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="I25" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="J25" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="K25" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="L25" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="M25" s="24"/>
+      <c r="AU25" s="25"/>
+    </row>
+    <row r="26" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="20">
+        <v>10.8</v>
+      </c>
+      <c r="C26" s="12">
+        <v>1</v>
+      </c>
+      <c r="D26" s="13">
+        <v>45811</v>
+      </c>
+      <c r="E26" s="13">
+        <v>45812</v>
+      </c>
+      <c r="F26" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="G26" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="H26" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="I26" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="J26" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="K26" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="L26" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="M26" s="24"/>
+      <c r="AU26" s="25"/>
+    </row>
+    <row r="27" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="20">
+        <v>10.8</v>
+      </c>
+      <c r="C27" s="12">
+        <v>1</v>
+      </c>
+      <c r="D27" s="13">
+        <v>45813</v>
+      </c>
+      <c r="E27" s="13">
+        <v>45813</v>
+      </c>
+      <c r="F27" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="G27" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="H27" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="I27" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="J27" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="K27" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="L27" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="M27" s="24"/>
+      <c r="AU27" s="25"/>
+    </row>
+    <row r="28" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="20">
+        <v>10.8</v>
+      </c>
+      <c r="C28" s="12">
+        <v>1</v>
+      </c>
+      <c r="D28" s="13">
+        <v>45813</v>
+      </c>
+      <c r="E28" s="13">
+        <v>45813</v>
+      </c>
+      <c r="F28" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="G28" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="H28" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="I28" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="J28" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="K28" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="L28" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="M28" s="24"/>
+      <c r="AU28" s="25"/>
+    </row>
+    <row r="29" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="20">
+        <v>10.8</v>
+      </c>
+      <c r="C29" s="12">
+        <v>1</v>
+      </c>
+      <c r="D29" s="13">
+        <v>45814</v>
+      </c>
+      <c r="E29" s="13">
+        <v>45820</v>
+      </c>
+      <c r="F29" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="G29" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="H29" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="I29" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="J29" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="K29" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="L29" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="M29" s="24"/>
+      <c r="AU29" s="25"/>
+    </row>
+    <row r="30" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="20">
+        <v>10.8</v>
+      </c>
+      <c r="C30" s="12">
+        <v>1</v>
+      </c>
+      <c r="D30" s="13">
+        <v>45815</v>
+      </c>
+      <c r="E30" s="13">
+        <v>45815</v>
+      </c>
+      <c r="F30" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="G30" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="H30" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="I30" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="J30" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="K30" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="L30" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="M30" s="24"/>
+      <c r="AU30" s="25"/>
+    </row>
+    <row r="31" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="20">
+        <v>10.8</v>
+      </c>
+      <c r="C31" s="12">
+        <v>1</v>
+      </c>
+      <c r="D31" s="13">
+        <v>45815</v>
+      </c>
+      <c r="E31" s="13">
         <v>45816</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="41"/>
-      <c r="O15" s="41"/>
-      <c r="P15" s="41"/>
-      <c r="Q15" s="41"/>
-      <c r="R15" s="41"/>
-      <c r="S15" s="41"/>
-      <c r="T15" s="41"/>
-      <c r="U15" s="41"/>
-      <c r="V15" s="41"/>
-      <c r="W15" s="41"/>
-      <c r="X15" s="41"/>
-      <c r="Y15" s="41"/>
-      <c r="Z15" s="41"/>
-      <c r="AA15" s="41"/>
-      <c r="AB15" s="41"/>
-      <c r="AC15" s="41"/>
-      <c r="AD15" s="41"/>
-      <c r="AE15" s="41"/>
-      <c r="AF15" s="41"/>
-      <c r="AG15" s="41"/>
-      <c r="AH15" s="41"/>
-      <c r="AI15" s="41"/>
-      <c r="AJ15" s="41"/>
-      <c r="AK15" s="41"/>
-      <c r="AL15" s="41"/>
-      <c r="AM15" s="41"/>
-      <c r="AN15" s="41"/>
-      <c r="AO15" s="41"/>
-      <c r="AP15" s="41"/>
-      <c r="AQ15" s="41"/>
-      <c r="AR15" s="41"/>
-      <c r="AS15" s="41"/>
-      <c r="AT15" s="41"/>
-      <c r="AU15" s="43"/>
+      <c r="F31" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="G31" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="H31" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="I31" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="J31" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="K31" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="L31" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="M31" s="24"/>
+      <c r="AU31" s="25"/>
     </row>
-    <row r="16" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="47" t="s">
+    <row r="32" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="20">
+        <v>10.8</v>
+      </c>
+      <c r="C32" s="12">
+        <v>1</v>
+      </c>
+      <c r="D32" s="13">
+        <v>45816</v>
+      </c>
+      <c r="E32" s="13">
+        <v>45816</v>
+      </c>
+      <c r="F32" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="G32" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="H32" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="I32" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="J32" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="K32" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="L32" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="M32" s="24"/>
+      <c r="AU32" s="25"/>
+    </row>
+    <row r="33" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="20">
+        <v>10.8</v>
+      </c>
+      <c r="C33" s="12">
+        <v>1</v>
+      </c>
+      <c r="D33" s="13">
+        <v>45815</v>
+      </c>
+      <c r="E33" s="13">
+        <v>45815</v>
+      </c>
+      <c r="F33" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="G33" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="H33" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="I33" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="J33" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="K33" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="L33" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="M33" s="24"/>
+      <c r="AU33" s="25"/>
+    </row>
+    <row r="34" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="20">
+        <v>10.8</v>
+      </c>
+      <c r="C34" s="12">
+        <v>1</v>
+      </c>
+      <c r="D34" s="13">
+        <v>45818</v>
+      </c>
+      <c r="E34" s="13">
+        <v>45818</v>
+      </c>
+      <c r="F34" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="G34" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="H34" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="I34" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="J34" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="K34" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="L34" s="11" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="M34" s="24"/>
+      <c r="AU34" s="25"/>
+    </row>
+    <row r="35" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="19">
+        <v>3</v>
+      </c>
+      <c r="C35" s="12">
+        <v>1</v>
+      </c>
+      <c r="D35" s="13">
+        <v>45805</v>
+      </c>
+      <c r="E35" s="13">
+        <v>45820</v>
+      </c>
+      <c r="F35" s="11" t="str">
+        <f t="shared" ref="F35:L35" ca="1" si="17">IF(AND(F$5&gt;$E35,$C35&lt;100%,F$5&lt;=TODAY()),"D","")</f>
+        <v/>
+      </c>
+      <c r="G35" s="11" t="str">
+        <f t="shared" ca="1" si="17"/>
+        <v/>
+      </c>
+      <c r="H35" s="11" t="str">
+        <f t="shared" ca="1" si="17"/>
+        <v/>
+      </c>
+      <c r="I35" s="11" t="str">
+        <f t="shared" ca="1" si="17"/>
+        <v/>
+      </c>
+      <c r="J35" s="11" t="str">
+        <f t="shared" ca="1" si="17"/>
+        <v/>
+      </c>
+      <c r="K35" s="11" t="str">
+        <f t="shared" ca="1" si="17"/>
+        <v/>
+      </c>
+      <c r="L35" s="11" t="str">
+        <f t="shared" ca="1" si="17"/>
+        <v/>
+      </c>
+      <c r="M35" s="24"/>
+      <c r="AU35" s="25"/>
+    </row>
+    <row r="36" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="48"/>
-      <c r="C16" s="49">
-        <v>0</v>
-      </c>
-      <c r="D16" s="50">
+      <c r="B36" s="19">
+        <v>3</v>
+      </c>
+      <c r="C36" s="12">
+        <v>1</v>
+      </c>
+      <c r="D36" s="13">
+        <v>45805</v>
+      </c>
+      <c r="E36" s="13">
+        <v>45805</v>
+      </c>
+      <c r="F36" s="11" t="str">
+        <f t="shared" ref="F36:L36" ca="1" si="18">IF(AND(F$5&gt;$E36,$C36&lt;100%,F$5&lt;=TODAY()),"D","")</f>
+        <v/>
+      </c>
+      <c r="G36" s="11" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v/>
+      </c>
+      <c r="H36" s="11" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v/>
+      </c>
+      <c r="I36" s="11" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v/>
+      </c>
+      <c r="J36" s="11" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v/>
+      </c>
+      <c r="K36" s="11" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v/>
+      </c>
+      <c r="L36" s="11" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v/>
+      </c>
+      <c r="M36" s="24"/>
+      <c r="AU36" s="25"/>
+    </row>
+    <row r="37" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="19"/>
+      <c r="C37" s="12">
+        <v>1</v>
+      </c>
+      <c r="D37" s="13">
+        <v>45807</v>
+      </c>
+      <c r="E37" s="13">
+        <v>45807</v>
+      </c>
+      <c r="M37" s="24"/>
+      <c r="AU37" s="25"/>
+    </row>
+    <row r="38" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="19"/>
+      <c r="C38" s="12">
+        <v>1</v>
+      </c>
+      <c r="D38" s="13">
         <v>45810</v>
       </c>
-      <c r="E16" s="50">
+      <c r="E38" s="13">
         <v>45810</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="44"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="45"/>
-      <c r="S16" s="45"/>
-      <c r="T16" s="45"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="45"/>
-      <c r="W16" s="45"/>
-      <c r="X16" s="45"/>
-      <c r="Y16" s="45"/>
-      <c r="Z16" s="45"/>
-      <c r="AA16" s="45"/>
-      <c r="AB16" s="45"/>
-      <c r="AC16" s="45"/>
-      <c r="AD16" s="45"/>
-      <c r="AE16" s="45"/>
-      <c r="AF16" s="45"/>
-      <c r="AG16" s="45"/>
-      <c r="AH16" s="45"/>
-      <c r="AI16" s="45"/>
-      <c r="AJ16" s="45"/>
-      <c r="AK16" s="45"/>
-      <c r="AL16" s="45"/>
-      <c r="AM16" s="45"/>
-      <c r="AN16" s="45"/>
-      <c r="AO16" s="45"/>
-      <c r="AP16" s="45"/>
-      <c r="AQ16" s="45"/>
-      <c r="AR16" s="45"/>
-      <c r="AS16" s="45"/>
-      <c r="AT16" s="45"/>
-      <c r="AU16" s="46"/>
+      <c r="M38" s="24"/>
+      <c r="AU38" s="25"/>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-      <c r="T17" s="17"/>
-      <c r="U17" s="17"/>
-      <c r="V17" s="17"/>
-      <c r="W17" s="17"/>
-      <c r="X17" s="17"/>
-      <c r="Y17" s="17"/>
-      <c r="Z17" s="17"/>
-      <c r="AA17" s="17"/>
-      <c r="AB17" s="17"/>
-      <c r="AC17" s="17"/>
-      <c r="AD17" s="17"/>
-      <c r="AE17" s="17"/>
-      <c r="AF17" s="17"/>
-      <c r="AG17" s="17"/>
-      <c r="AH17" s="17"/>
-      <c r="AI17" s="17"/>
-      <c r="AJ17" s="17"/>
-      <c r="AK17" s="17"/>
-      <c r="AL17" s="17"/>
-      <c r="AM17" s="17"/>
-      <c r="AN17" s="17"/>
-      <c r="AO17" s="17"/>
-      <c r="AP17" s="17"/>
-      <c r="AQ17" s="17"/>
-      <c r="AR17" s="17"/>
-      <c r="AS17" s="17"/>
-      <c r="AT17" s="17"/>
-      <c r="AU17" s="17"/>
+    <row r="39" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="19">
+        <v>1</v>
+      </c>
+      <c r="C39" s="12">
+        <v>1</v>
+      </c>
+      <c r="D39" s="13">
+        <v>45811</v>
+      </c>
+      <c r="E39" s="13">
+        <v>45811</v>
+      </c>
+      <c r="M39" s="24"/>
+      <c r="AU39" s="25"/>
+    </row>
+    <row r="40" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="19">
+        <v>1</v>
+      </c>
+      <c r="C40" s="12">
+        <v>1</v>
+      </c>
+      <c r="D40" s="13">
+        <v>45811</v>
+      </c>
+      <c r="E40" s="13">
+        <v>45819</v>
+      </c>
+      <c r="M40" s="24"/>
+      <c r="AU40" s="25"/>
+    </row>
+    <row r="41" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="19">
+        <v>1</v>
+      </c>
+      <c r="C41" s="12">
+        <v>1</v>
+      </c>
+      <c r="D41" s="13">
+        <v>45812</v>
+      </c>
+      <c r="E41" s="13">
+        <v>45812</v>
+      </c>
+      <c r="M41" s="24"/>
+      <c r="AU41" s="25"/>
+    </row>
+    <row r="42" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="19">
+        <v>1</v>
+      </c>
+      <c r="C42" s="12">
+        <v>1</v>
+      </c>
+      <c r="D42" s="13">
+        <v>45812</v>
+      </c>
+      <c r="E42" s="13">
+        <v>45813</v>
+      </c>
+      <c r="M42" s="24"/>
+      <c r="AU42" s="25"/>
+    </row>
+    <row r="43" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="19">
+        <v>1</v>
+      </c>
+      <c r="C43" s="12">
+        <v>1</v>
+      </c>
+      <c r="D43" s="13">
+        <v>45813</v>
+      </c>
+      <c r="E43" s="13">
+        <v>45813</v>
+      </c>
+      <c r="M43" s="24"/>
+      <c r="AU43" s="25"/>
+    </row>
+    <row r="44" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" s="19">
+        <v>1</v>
+      </c>
+      <c r="C44" s="12">
+        <v>1</v>
+      </c>
+      <c r="D44" s="13">
+        <v>45814</v>
+      </c>
+      <c r="E44" s="13">
+        <v>45814</v>
+      </c>
+      <c r="M44" s="24"/>
+      <c r="AU44" s="25"/>
+    </row>
+    <row r="45" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" s="19">
+        <v>1</v>
+      </c>
+      <c r="C45" s="12">
+        <v>1</v>
+      </c>
+      <c r="D45" s="13">
+        <v>45814</v>
+      </c>
+      <c r="E45" s="13">
+        <v>45816</v>
+      </c>
+      <c r="M45" s="24"/>
+      <c r="AU45" s="25"/>
+    </row>
+    <row r="46" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" s="19">
+        <v>1</v>
+      </c>
+      <c r="C46" s="12">
+        <v>1</v>
+      </c>
+      <c r="D46" s="13">
+        <v>45818</v>
+      </c>
+      <c r="E46" s="13">
+        <v>45818</v>
+      </c>
+      <c r="M46" s="24"/>
+      <c r="AU46" s="25"/>
+    </row>
+    <row r="47" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="19"/>
+      <c r="C47" s="47">
+        <v>1</v>
+      </c>
+      <c r="D47" s="55">
+        <v>45810</v>
+      </c>
+      <c r="E47" s="54">
+        <v>45819</v>
+      </c>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="41"/>
+      <c r="N47" s="40"/>
+      <c r="O47" s="40"/>
+      <c r="P47" s="40"/>
+      <c r="Q47" s="40"/>
+      <c r="R47" s="40"/>
+      <c r="S47" s="40"/>
+      <c r="T47" s="40"/>
+      <c r="U47" s="40"/>
+      <c r="V47" s="40"/>
+      <c r="W47" s="40"/>
+      <c r="X47" s="40"/>
+      <c r="Y47" s="40"/>
+      <c r="Z47" s="40"/>
+      <c r="AA47" s="40"/>
+      <c r="AB47" s="40"/>
+      <c r="AC47" s="40"/>
+      <c r="AD47" s="40"/>
+      <c r="AE47" s="40"/>
+      <c r="AF47" s="40"/>
+      <c r="AG47" s="40"/>
+      <c r="AH47" s="40"/>
+      <c r="AI47" s="40"/>
+      <c r="AJ47" s="40"/>
+      <c r="AK47" s="40"/>
+      <c r="AL47" s="40"/>
+      <c r="AM47" s="40"/>
+      <c r="AN47" s="40"/>
+      <c r="AO47" s="40"/>
+      <c r="AP47" s="40"/>
+      <c r="AQ47" s="40"/>
+      <c r="AR47" s="40"/>
+      <c r="AS47" s="40"/>
+      <c r="AT47" s="40"/>
+      <c r="AU47" s="42"/>
+    </row>
+    <row r="48" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="52"/>
+      <c r="C48" s="53">
+        <v>1</v>
+      </c>
+      <c r="D48" s="54">
+        <v>45810</v>
+      </c>
+      <c r="E48" s="54">
+        <v>45810</v>
+      </c>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="26"/>
+      <c r="K48" s="26"/>
+      <c r="L48" s="26"/>
+      <c r="M48" s="41"/>
+      <c r="N48" s="40"/>
+      <c r="O48" s="40"/>
+      <c r="P48" s="40"/>
+      <c r="Q48" s="40"/>
+      <c r="R48" s="40"/>
+      <c r="S48" s="40"/>
+      <c r="T48" s="40"/>
+      <c r="U48" s="40"/>
+      <c r="V48" s="40"/>
+      <c r="W48" s="40"/>
+      <c r="X48" s="40"/>
+      <c r="Y48" s="40"/>
+      <c r="Z48" s="40"/>
+      <c r="AA48" s="40"/>
+      <c r="AB48" s="40"/>
+      <c r="AC48" s="40"/>
+      <c r="AD48" s="40"/>
+      <c r="AE48" s="40"/>
+      <c r="AF48" s="40"/>
+      <c r="AG48" s="40"/>
+      <c r="AH48" s="40"/>
+      <c r="AI48" s="40"/>
+      <c r="AJ48" s="40"/>
+      <c r="AK48" s="40"/>
+      <c r="AL48" s="40"/>
+      <c r="AM48" s="40"/>
+      <c r="AN48" s="40"/>
+      <c r="AO48" s="40"/>
+      <c r="AP48" s="40"/>
+      <c r="AQ48" s="40"/>
+      <c r="AR48" s="40"/>
+      <c r="AS48" s="40"/>
+      <c r="AT48" s="40"/>
+      <c r="AU48" s="42"/>
+    </row>
+    <row r="49" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="52"/>
+      <c r="C49" s="53">
+        <v>1</v>
+      </c>
+      <c r="D49" s="54">
+        <v>45811</v>
+      </c>
+      <c r="E49" s="54">
+        <v>45811</v>
+      </c>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="26"/>
+      <c r="K49" s="26"/>
+      <c r="L49" s="26"/>
+      <c r="M49" s="41"/>
+      <c r="N49" s="40"/>
+      <c r="O49" s="40"/>
+      <c r="P49" s="40"/>
+      <c r="Q49" s="40"/>
+      <c r="R49" s="40"/>
+      <c r="S49" s="40"/>
+      <c r="T49" s="40"/>
+      <c r="U49" s="40"/>
+      <c r="V49" s="40"/>
+      <c r="W49" s="40"/>
+      <c r="X49" s="40"/>
+      <c r="Y49" s="40"/>
+      <c r="Z49" s="40"/>
+      <c r="AA49" s="40"/>
+      <c r="AB49" s="40"/>
+      <c r="AC49" s="40"/>
+      <c r="AD49" s="40"/>
+      <c r="AE49" s="40"/>
+      <c r="AF49" s="40"/>
+      <c r="AG49" s="40"/>
+      <c r="AH49" s="40"/>
+      <c r="AI49" s="40"/>
+      <c r="AJ49" s="40"/>
+      <c r="AK49" s="40"/>
+      <c r="AL49" s="40"/>
+      <c r="AM49" s="40"/>
+      <c r="AN49" s="40"/>
+      <c r="AO49" s="40"/>
+      <c r="AP49" s="40"/>
+      <c r="AQ49" s="40"/>
+      <c r="AR49" s="40"/>
+      <c r="AS49" s="40"/>
+      <c r="AT49" s="40"/>
+      <c r="AU49" s="42"/>
+    </row>
+    <row r="50" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" s="52"/>
+      <c r="C50" s="53">
+        <v>1</v>
+      </c>
+      <c r="D50" s="54">
+        <v>45811</v>
+      </c>
+      <c r="E50" s="54">
+        <v>45811</v>
+      </c>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="26"/>
+      <c r="K50" s="26"/>
+      <c r="L50" s="26"/>
+      <c r="M50" s="41"/>
+      <c r="N50" s="40"/>
+      <c r="O50" s="40"/>
+      <c r="P50" s="40"/>
+      <c r="Q50" s="40"/>
+      <c r="R50" s="40"/>
+      <c r="S50" s="40"/>
+      <c r="T50" s="40"/>
+      <c r="U50" s="40"/>
+      <c r="V50" s="40"/>
+      <c r="W50" s="40"/>
+      <c r="X50" s="40"/>
+      <c r="Y50" s="40"/>
+      <c r="Z50" s="40"/>
+      <c r="AA50" s="40"/>
+      <c r="AB50" s="40"/>
+      <c r="AC50" s="40"/>
+      <c r="AD50" s="40"/>
+      <c r="AE50" s="40"/>
+      <c r="AF50" s="40"/>
+      <c r="AG50" s="40"/>
+      <c r="AH50" s="40"/>
+      <c r="AI50" s="40"/>
+      <c r="AJ50" s="40"/>
+      <c r="AK50" s="40"/>
+      <c r="AL50" s="40"/>
+      <c r="AM50" s="40"/>
+      <c r="AN50" s="40"/>
+      <c r="AO50" s="40"/>
+      <c r="AP50" s="40"/>
+      <c r="AQ50" s="40"/>
+      <c r="AR50" s="40"/>
+      <c r="AS50" s="40"/>
+      <c r="AT50" s="40"/>
+      <c r="AU50" s="42"/>
+    </row>
+    <row r="51" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="52"/>
+      <c r="C51" s="53">
+        <v>1</v>
+      </c>
+      <c r="D51" s="54">
+        <v>45813</v>
+      </c>
+      <c r="E51" s="54">
+        <v>45819</v>
+      </c>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="26"/>
+      <c r="K51" s="26"/>
+      <c r="L51" s="26"/>
+      <c r="M51" s="41"/>
+      <c r="N51" s="40"/>
+      <c r="O51" s="40"/>
+      <c r="P51" s="40"/>
+      <c r="Q51" s="40"/>
+      <c r="R51" s="40"/>
+      <c r="S51" s="40"/>
+      <c r="T51" s="40"/>
+      <c r="U51" s="40"/>
+      <c r="V51" s="40"/>
+      <c r="W51" s="40"/>
+      <c r="X51" s="40"/>
+      <c r="Y51" s="40"/>
+      <c r="Z51" s="40"/>
+      <c r="AA51" s="40"/>
+      <c r="AB51" s="40"/>
+      <c r="AC51" s="40"/>
+      <c r="AD51" s="40"/>
+      <c r="AE51" s="40"/>
+      <c r="AF51" s="40"/>
+      <c r="AG51" s="40"/>
+      <c r="AH51" s="40"/>
+      <c r="AI51" s="40"/>
+      <c r="AJ51" s="40"/>
+      <c r="AK51" s="40"/>
+      <c r="AL51" s="40"/>
+      <c r="AM51" s="40"/>
+      <c r="AN51" s="40"/>
+      <c r="AO51" s="40"/>
+      <c r="AP51" s="40"/>
+      <c r="AQ51" s="40"/>
+      <c r="AR51" s="40"/>
+      <c r="AS51" s="40"/>
+      <c r="AT51" s="40"/>
+      <c r="AU51" s="42"/>
+    </row>
+    <row r="52" spans="1:47" s="11" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="49"/>
+      <c r="C52" s="50">
+        <v>1</v>
+      </c>
+      <c r="D52" s="51">
+        <v>45814</v>
+      </c>
+      <c r="E52" s="51">
+        <v>45816</v>
+      </c>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="26"/>
+      <c r="K52" s="26"/>
+      <c r="L52" s="26"/>
+      <c r="M52" s="43"/>
+      <c r="N52" s="44"/>
+      <c r="O52" s="44"/>
+      <c r="P52" s="44"/>
+      <c r="Q52" s="44"/>
+      <c r="R52" s="44"/>
+      <c r="S52" s="44"/>
+      <c r="T52" s="44"/>
+      <c r="U52" s="44"/>
+      <c r="V52" s="44"/>
+      <c r="W52" s="44"/>
+      <c r="X52" s="44"/>
+      <c r="Y52" s="44"/>
+      <c r="Z52" s="44"/>
+      <c r="AA52" s="44"/>
+      <c r="AB52" s="44"/>
+      <c r="AC52" s="44"/>
+      <c r="AD52" s="44"/>
+      <c r="AE52" s="44"/>
+      <c r="AF52" s="44"/>
+      <c r="AG52" s="44"/>
+      <c r="AH52" s="44"/>
+      <c r="AI52" s="44"/>
+      <c r="AJ52" s="44"/>
+      <c r="AK52" s="44"/>
+      <c r="AL52" s="44"/>
+      <c r="AM52" s="44"/>
+      <c r="AN52" s="44"/>
+      <c r="AO52" s="44"/>
+      <c r="AP52" s="44"/>
+      <c r="AQ52" s="44"/>
+      <c r="AR52" s="44"/>
+      <c r="AS52" s="44"/>
+      <c r="AT52" s="44"/>
+      <c r="AU52" s="45"/>
+    </row>
+    <row r="53" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A53" s="17"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="17"/>
+      <c r="L53" s="17"/>
+      <c r="M53" s="17"/>
+      <c r="N53" s="17"/>
+      <c r="O53" s="17"/>
+      <c r="P53" s="17"/>
+      <c r="Q53" s="17"/>
+      <c r="R53" s="17"/>
+      <c r="S53" s="17"/>
+      <c r="T53" s="17"/>
+      <c r="U53" s="17"/>
+      <c r="V53" s="17"/>
+      <c r="W53" s="17"/>
+      <c r="X53" s="17"/>
+      <c r="Y53" s="17"/>
+      <c r="Z53" s="17"/>
+      <c r="AA53" s="17"/>
+      <c r="AB53" s="17"/>
+      <c r="AC53" s="17"/>
+      <c r="AD53" s="17"/>
+      <c r="AE53" s="17"/>
+      <c r="AF53" s="17"/>
+      <c r="AG53" s="17"/>
+      <c r="AH53" s="17"/>
+      <c r="AI53" s="17"/>
+      <c r="AJ53" s="17"/>
+      <c r="AK53" s="17"/>
+      <c r="AL53" s="17"/>
+      <c r="AM53" s="17"/>
+      <c r="AN53" s="17"/>
+      <c r="AO53" s="17"/>
+      <c r="AP53" s="17"/>
+      <c r="AQ53" s="17"/>
+      <c r="AR53" s="17"/>
+      <c r="AS53" s="17"/>
+      <c r="AT53" s="17"/>
+      <c r="AU53" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2853,209 +4985,229 @@
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="O2:Q2"/>
   </mergeCells>
-  <conditionalFormatting sqref="C4:AN6 C7 F7:AN7 C16:AU16 C12:AU14 AO4:AU7 C11 E11:AU11">
-    <cfRule type="expression" dxfId="40" priority="41">
+  <conditionalFormatting sqref="A6:B6 C25:D34 F27:AU34 C35:AU52 C7:E23">
+    <cfRule type="expression" dxfId="48" priority="90">
+      <formula>AND(today&gt;=A$5,today&lt;A$5+1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24:AU24">
+    <cfRule type="expression" dxfId="47" priority="58">
       <formula>AND(today&gt;=C$5,today&lt;C$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11:AU14 F16:AU16 F7:AU7">
-    <cfRule type="expression" dxfId="39" priority="84" stopIfTrue="1">
+  <conditionalFormatting sqref="F7:AN23">
+    <cfRule type="expression" dxfId="46" priority="63">
+      <formula>AND(task_start&lt;=F$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=F$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24:AN34">
+    <cfRule type="expression" dxfId="45" priority="54">
+      <formula>AND(task_start&lt;=F$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=F$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="55" stopIfTrue="1">
+      <formula>AND(task_end&gt;=F$5,task_start&lt;F$5+1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F52:AN52">
+    <cfRule type="expression" dxfId="43" priority="67">
+      <formula>AND(task_start&lt;=F$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=F$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7:AU7 F25:AU52">
+    <cfRule type="expression" dxfId="42" priority="136" stopIfTrue="1">
       <formula>COUNTIF(holidays,F$5)&gt;=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F12:AU14 AO16:AU16">
-    <cfRule type="expression" dxfId="38" priority="86" stopIfTrue="1">
+  <conditionalFormatting sqref="AO24:AU34 F7:AU23">
+    <cfRule type="expression" dxfId="41" priority="64" stopIfTrue="1">
       <formula>AND(task_end&gt;=F$5,task_start&lt;F$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AO11:AU11 F7:AU7">
-    <cfRule type="expression" dxfId="37" priority="40" stopIfTrue="1">
+  <conditionalFormatting sqref="F15:AU23">
+    <cfRule type="expression" dxfId="40" priority="65">
+      <formula>AND(today&gt;=F$5,today&lt;F$5+1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="66" stopIfTrue="1">
+      <formula>COUNTIF(holidays,F$5)&gt;=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24:AU24">
+    <cfRule type="expression" dxfId="38" priority="59" stopIfTrue="1">
+      <formula>COUNTIF(holidays,F$5)&gt;=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO52:AU52 F35:AU51">
+    <cfRule type="expression" dxfId="37" priority="137">
+      <formula>AND(task_start&lt;=F$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=F$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="138" stopIfTrue="1">
       <formula>AND(task_end&gt;=F$5,task_start&lt;F$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7:AN7">
-    <cfRule type="expression" dxfId="36" priority="39">
+  <conditionalFormatting sqref="F52:BC52">
+    <cfRule type="expression" dxfId="35" priority="68" stopIfTrue="1">
+      <formula>AND(task_end&gt;=F$5,task_start&lt;F$5+1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO4:AU7 F7:AN7 C4:AN6">
+    <cfRule type="expression" dxfId="34" priority="93">
+      <formula>AND(today&gt;=C$5,today&lt;C$5+1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO7:AU34">
+    <cfRule type="expression" dxfId="33" priority="56">
+      <formula>AND(task_start&lt;=AO$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=AO$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F47:AN47">
+    <cfRule type="expression" dxfId="32" priority="45">
       <formula>AND(task_start&lt;=F$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=F$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F12:AU14 AO16:AU16">
-    <cfRule type="expression" dxfId="35" priority="85">
+  <conditionalFormatting sqref="F47:BC47">
+    <cfRule type="expression" dxfId="31" priority="46" stopIfTrue="1">
+      <formula>AND(task_end&gt;=F$5,task_start&lt;F$5+1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F48:AN48">
+    <cfRule type="expression" dxfId="30" priority="43">
       <formula>AND(task_start&lt;=F$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=F$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:B6">
-    <cfRule type="expression" dxfId="34" priority="38">
-      <formula>AND(today&gt;=A$5,today&lt;A$5+1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO11:AU11 AO7:AU7">
-    <cfRule type="expression" dxfId="33" priority="34">
-      <formula>AND(task_start&lt;=AO$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=AO$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F11:AN11">
-    <cfRule type="expression" dxfId="32" priority="33" stopIfTrue="1">
+  <conditionalFormatting sqref="F48:BC48">
+    <cfRule type="expression" dxfId="29" priority="44" stopIfTrue="1">
       <formula>AND(task_end&gt;=F$5,task_start&lt;F$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11:AN11">
-    <cfRule type="expression" dxfId="31" priority="32">
+  <conditionalFormatting sqref="F49:AN49">
+    <cfRule type="expression" dxfId="28" priority="41">
       <formula>AND(task_start&lt;=F$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=F$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16:AN16">
-    <cfRule type="expression" dxfId="30" priority="30">
+  <conditionalFormatting sqref="F49:BC49">
+    <cfRule type="expression" dxfId="27" priority="42" stopIfTrue="1">
+      <formula>AND(task_end&gt;=F$5,task_start&lt;F$5+1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F50:AN50">
+    <cfRule type="expression" dxfId="26" priority="39">
       <formula>AND(task_start&lt;=F$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=F$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16:BC16">
-    <cfRule type="expression" dxfId="29" priority="31" stopIfTrue="1">
+  <conditionalFormatting sqref="F50:BC50">
+    <cfRule type="expression" dxfId="25" priority="40" stopIfTrue="1">
       <formula>AND(task_end&gt;=F$5,task_start&lt;F$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
-    <cfRule type="expression" dxfId="28" priority="21">
-      <formula>AND(today&gt;=E$5,today&lt;E$5+1)</formula>
+  <conditionalFormatting sqref="F51:AN51">
+    <cfRule type="expression" dxfId="24" priority="35">
+      <formula>AND(task_start&lt;=F$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=F$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9 F9:AU9">
-    <cfRule type="expression" dxfId="27" priority="28">
-      <formula>AND(today&gt;=C$5,today&lt;C$5+1)</formula>
+  <conditionalFormatting sqref="F51:BC51">
+    <cfRule type="expression" dxfId="23" priority="36" stopIfTrue="1">
+      <formula>AND(task_end&gt;=F$5,task_start&lt;F$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F9:AU9">
-    <cfRule type="expression" dxfId="26" priority="29" stopIfTrue="1">
+  <conditionalFormatting sqref="F8:AU8">
+    <cfRule type="expression" dxfId="22" priority="31">
+      <formula>AND(today&gt;=F$5,today&lt;F$5+1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="32" stopIfTrue="1">
       <formula>COUNTIF(holidays,F$5)&gt;=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:AU9">
-    <cfRule type="expression" dxfId="25" priority="27" stopIfTrue="1">
-      <formula>AND(task_end&gt;=F$5,task_start&lt;F$5+1)</formula>
+    <cfRule type="expression" dxfId="20" priority="29">
+      <formula>AND(today&gt;=F$5,today&lt;F$5+1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="30" stopIfTrue="1">
+      <formula>COUNTIF(holidays,F$5)&gt;=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F9:AN9">
-    <cfRule type="expression" dxfId="24" priority="26">
-      <formula>AND(task_start&lt;=F$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=F$5)</formula>
+  <conditionalFormatting sqref="F10:AU10">
+    <cfRule type="expression" dxfId="18" priority="27">
+      <formula>AND(today&gt;=F$5,today&lt;F$5+1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="28" stopIfTrue="1">
+      <formula>COUNTIF(holidays,F$5)&gt;=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AO9:AU9">
-    <cfRule type="expression" dxfId="23" priority="25">
-      <formula>AND(task_start&lt;=AO$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=AO$5)</formula>
+  <conditionalFormatting sqref="F14:AU14">
+    <cfRule type="expression" dxfId="16" priority="25">
+      <formula>AND(today&gt;=F$5,today&lt;F$5+1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="26" stopIfTrue="1">
+      <formula>COUNTIF(holidays,F$5)&gt;=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="22" priority="24">
-      <formula>AND(today&gt;=D$5,today&lt;D$5+1)</formula>
+  <conditionalFormatting sqref="F13:AU13">
+    <cfRule type="expression" dxfId="14" priority="23">
+      <formula>AND(today&gt;=F$5,today&lt;F$5+1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="24" stopIfTrue="1">
+      <formula>COUNTIF(holidays,F$5)&gt;=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9">
-    <cfRule type="expression" dxfId="21" priority="23">
+  <conditionalFormatting sqref="F12:AU12">
+    <cfRule type="expression" dxfId="12" priority="21">
+      <formula>AND(today&gt;=F$5,today&lt;F$5+1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="22" stopIfTrue="1">
+      <formula>COUNTIF(holidays,F$5)&gt;=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11:AU11">
+    <cfRule type="expression" dxfId="10" priority="19">
+      <formula>AND(today&gt;=F$5,today&lt;F$5+1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="20" stopIfTrue="1">
+      <formula>COUNTIF(holidays,F$5)&gt;=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25:AU26">
+    <cfRule type="expression" dxfId="8" priority="17">
       <formula>AND(today&gt;=E$5,today&lt;E$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="20" priority="22">
-      <formula>AND(today&gt;=D$5,today&lt;D$5+1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15:AU15">
-    <cfRule type="expression" dxfId="19" priority="17">
-      <formula>AND(today&gt;=C$5,today&lt;C$5+1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F15:AU15">
-    <cfRule type="expression" dxfId="18" priority="18" stopIfTrue="1">
-      <formula>COUNTIF(holidays,F$5)&gt;=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO15:AU15">
-    <cfRule type="expression" dxfId="17" priority="20" stopIfTrue="1">
-      <formula>AND(task_end&gt;=AO$5,task_start&lt;AO$5+1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO15:AU15">
-    <cfRule type="expression" dxfId="16" priority="19">
-      <formula>AND(task_start&lt;=AO$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=AO$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F15:AN15">
-    <cfRule type="expression" dxfId="15" priority="15">
-      <formula>AND(task_start&lt;=F$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=F$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F15:BC15">
-    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
-      <formula>AND(task_end&gt;=F$5,task_start&lt;F$5+1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8 F8:AU8">
-    <cfRule type="expression" dxfId="13" priority="13">
-      <formula>AND(today&gt;=C$5,today&lt;C$5+1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8:AU8">
-    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
-      <formula>COUNTIF(holidays,F$5)&gt;=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8:AU8">
-    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
-      <formula>AND(task_end&gt;=F$5,task_start&lt;F$5+1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8:AN8">
-    <cfRule type="expression" dxfId="10" priority="11">
-      <formula>AND(task_start&lt;=F$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=F$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO8:AU8">
-    <cfRule type="expression" dxfId="9" priority="10">
-      <formula>AND(task_start&lt;=AO$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=AO$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="expression" dxfId="8" priority="9">
-      <formula>AND(today&gt;=D$5,today&lt;D$5+1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="7" priority="8">
+  <conditionalFormatting sqref="E27">
+    <cfRule type="expression" dxfId="7" priority="14">
       <formula>AND(today&gt;=E$5,today&lt;E$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:AU10">
-    <cfRule type="expression" dxfId="6" priority="6">
-      <formula>AND(today&gt;=C$5,today&lt;C$5+1)</formula>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="expression" dxfId="6" priority="13">
+      <formula>AND(today&gt;=E$5,today&lt;E$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10:AU10">
-    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
-      <formula>COUNTIF(holidays,F$5)&gt;=1</formula>
+  <conditionalFormatting sqref="E29">
+    <cfRule type="expression" dxfId="5" priority="12">
+      <formula>AND(today&gt;=E$5,today&lt;E$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AO10:AU10">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
-      <formula>AND(task_end&gt;=AO$5,task_start&lt;AO$5+1)</formula>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="expression" dxfId="4" priority="10">
+      <formula>AND(today&gt;=E$5,today&lt;E$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AO10:AU10">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>AND(task_start&lt;=AO$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=AO$5)</formula>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="expression" dxfId="3" priority="9">
+      <formula>AND(today&gt;=E$5,today&lt;E$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10:AN10">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>AND(task_end&gt;=F$5,task_start&lt;F$5+1)</formula>
+  <conditionalFormatting sqref="E32">
+    <cfRule type="expression" dxfId="2" priority="7">
+      <formula>AND(today&gt;=E$5,today&lt;E$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10:AN10">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>AND(task_start&lt;=F$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=F$5)</formula>
+  <conditionalFormatting sqref="E33">
+    <cfRule type="expression" dxfId="1" priority="6">
+      <formula>AND(today&gt;=E$5,today&lt;E$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(today&gt;=D$5,today&lt;D$5+1)</formula>
+  <conditionalFormatting sqref="E34">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>AND(today&gt;=E$5,today&lt;E$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -3070,26 +5222,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="74c9d3ac-d6d8-447b-a665-09e0c2a2ccfe">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d70a3488-2cc6-4e72-88b9-773372669d74" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010012DD97B986BE724D84C7CC5C058BC951" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b9aa710d5afa1f84a3d5de9e1ba6cc8c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="74c9d3ac-d6d8-447b-a665-09e0c2a2ccfe" xmlns:ns3="d70a3488-2cc6-4e72-88b9-773372669d74" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7ca688a2f035e9871bd8f94df963a1f2" ns2:_="" ns3:_="">
     <xsd:import namespace="74c9d3ac-d6d8-447b-a665-09e0c2a2ccfe"/>
@@ -3290,26 +5422,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60E1F045-850F-4307-9AD2-CB5E333E1429}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="74c9d3ac-d6d8-447b-a665-09e0c2a2ccfe"/>
-    <ds:schemaRef ds:uri="d70a3488-2cc6-4e72-88b9-773372669d74"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="74c9d3ac-d6d8-447b-a665-09e0c2a2ccfe">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d70a3488-2cc6-4e72-88b9-773372669d74" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{711F0C19-C2EA-4E28-B13A-1B62D065ED34}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82D82954-9AC6-45FC-ABB0-4AF1F46D53DD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3328,6 +5461,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60E1F045-850F-4307-9AD2-CB5E333E1429}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="74c9d3ac-d6d8-447b-a665-09e0c2a2ccfe"/>
+    <ds:schemaRef ds:uri="d70a3488-2cc6-4e72-88b9-773372669d74"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{711F0C19-C2EA-4E28-B13A-1B62D065ED34}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{4b512a4e-bb54-4328-ad34-d43205aaa1ec}" enabled="1" method="Standard" siteId="{f01e930a-b52e-42b1-b70f-a8882b5d043b}" removed="0"/>

</xml_diff>